<commit_message>
created solution surface graph
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -72,6 +72,400 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gaussian Elimination</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gauss Seidel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="113454464"/>
+        <c:axId val="48047232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="113454464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="48047232"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48047232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="150"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113454464"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6248401" y="276226"/>
+          <a:ext cx="2124074" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Size of Mesh</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> vs. Time</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C24"/>
+  <dimension ref="A2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -384,31 +778,43 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -416,10 +822,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -427,10 +833,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -438,73 +844,93 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>133</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>659</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>75</v>
+      </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>80</v>
+      </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>85</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>90</v>
+      </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>95</v>
+      </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>100</v>
+      </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
@@ -531,13 +957,9 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>